<commit_message>
refactor project excel table, create uidata, data model and excel data;
</commit_message>
<xml_diff>
--- a/app/res/master timing chart_template.xlsx
+++ b/app/res/master timing chart_template.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="793" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="793" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="auto_property" sheetId="16" r:id="rId1"/>
     <sheet name="auto_tags" sheetId="15" r:id="rId2"/>
     <sheet name="auto_tasks" sheetId="21" r:id="rId3"/>
-    <sheet name="auto_task_mule" sheetId="17" r:id="rId4"/>
-    <sheet name="auto_task_hotissue" sheetId="22" r:id="rId5"/>
-    <sheet name="auto_task_ewo" sheetId="23" r:id="rId6"/>
-    <sheet name="auto_task_normal" sheetId="24" r:id="rId7"/>
+    <sheet name="auto_task_0" sheetId="17" r:id="rId4"/>
+    <sheet name="auto_task_1" sheetId="22" r:id="rId5"/>
+    <sheet name="auto_task_2" sheetId="23" r:id="rId6"/>
+    <sheet name="auto_task_3" sheetId="24" r:id="rId7"/>
     <sheet name="auto_snorkelnoise" sheetId="20" r:id="rId8"/>
     <sheet name="README" sheetId="19" r:id="rId9"/>
     <sheet name="MASTER TIMING" sheetId="12" r:id="rId10"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="129">
   <si>
     <t>J</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -168,10 +168,6 @@
   </si>
   <si>
     <t>Week</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -518,27 +514,7 @@
     <t>dB(A)</t>
   </si>
   <si>
-    <t>${auto_task_mule}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${auto_task_hotissue}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${auto_task_ewo}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${auto_task_normal}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>This is a Hotissue Task.</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>rootcause</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -579,6 +555,38 @@
   </si>
   <si>
     <t>This is a Normal Task.</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>${auto_task_0}</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>${auto_task_1}</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>${auto_task_2}</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>${auto_task_3}</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>sorp</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date(Sorp-Week)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date(Adjusted)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rootCause</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -985,6 +993,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1058,21 +1081,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -16227,28 +16235,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2">
         <v>258</v>
@@ -16256,7 +16265,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -16264,7 +16273,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -16272,10 +16281,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>83</v>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="23">
+        <v>42641</v>
       </c>
     </row>
   </sheetData>
@@ -16327,156 +16344,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:58" ht="36" customHeight="1">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
+      <c r="AS1" s="52"/>
+      <c r="AT1" s="52"/>
+      <c r="AU1" s="52"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="52"/>
+      <c r="AX1" s="52"/>
+      <c r="AY1" s="52"/>
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+    </row>
+    <row r="2" spans="2:58" ht="27" customHeight="1">
+      <c r="B2" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="60">
+        <v>2016</v>
+      </c>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="57">
+        <v>2017</v>
+      </c>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="59"/>
+      <c r="AP2" s="63">
+        <v>2018</v>
+      </c>
+      <c r="AQ2" s="64"/>
+      <c r="AR2" s="64"/>
+      <c r="AS2" s="64"/>
+      <c r="AT2" s="64"/>
+      <c r="AU2" s="64"/>
+      <c r="AV2" s="64"/>
+      <c r="AW2" s="64"/>
+      <c r="AX2" s="64"/>
+      <c r="AY2" s="64"/>
+      <c r="AZ2" s="64"/>
+      <c r="BA2" s="65"/>
+      <c r="BB2" s="66">
+        <v>2019</v>
+      </c>
+      <c r="BC2" s="67"/>
+      <c r="BD2" s="67"/>
+      <c r="BE2" s="67"/>
+      <c r="BF2" s="68"/>
+    </row>
+    <row r="3" spans="2:58">
+      <c r="B3" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="47"/>
-      <c r="AQ1" s="47"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="47"/>
-      <c r="AT1" s="47"/>
-      <c r="AU1" s="47"/>
-      <c r="AV1" s="47"/>
-      <c r="AW1" s="47"/>
-      <c r="AX1" s="47"/>
-      <c r="AY1" s="47"/>
-      <c r="AZ1" s="47"/>
-      <c r="BA1" s="47"/>
-      <c r="BB1" s="47"/>
-      <c r="BC1" s="47"/>
-      <c r="BD1" s="47"/>
-      <c r="BE1" s="47"/>
-      <c r="BF1" s="47"/>
-    </row>
-    <row r="2" spans="2:58" ht="27" customHeight="1">
-      <c r="B2" s="64" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="55">
-        <v>2016</v>
-      </c>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="57"/>
-      <c r="AD2" s="52">
-        <v>2017</v>
-      </c>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="58">
-        <v>2018</v>
-      </c>
-      <c r="AQ2" s="59"/>
-      <c r="AR2" s="59"/>
-      <c r="AS2" s="59"/>
-      <c r="AT2" s="59"/>
-      <c r="AU2" s="59"/>
-      <c r="AV2" s="59"/>
-      <c r="AW2" s="59"/>
-      <c r="AX2" s="59"/>
-      <c r="AY2" s="59"/>
-      <c r="AZ2" s="59"/>
-      <c r="BA2" s="60"/>
-      <c r="BB2" s="61">
-        <v>2019</v>
-      </c>
-      <c r="BC2" s="62"/>
-      <c r="BD2" s="62"/>
-      <c r="BE2" s="62"/>
-      <c r="BF2" s="63"/>
-    </row>
-    <row r="3" spans="2:58">
-      <c r="B3" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="24" t="s">
+      <c r="I3" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="24" t="s">
-        <v>72</v>
-      </c>
       <c r="J3" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="24" t="s">
         <v>20</v>
@@ -16624,73 +16641,73 @@
       </c>
     </row>
     <row r="4" spans="2:58" ht="45" customHeight="1">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="75"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="75"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="75"/>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="75"/>
-      <c r="AC4" s="75"/>
-      <c r="AD4" s="75"/>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="75"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="75"/>
-      <c r="AK4" s="75"/>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="75"/>
-      <c r="AN4" s="75"/>
-      <c r="AO4" s="75"/>
-      <c r="AP4" s="75"/>
-      <c r="AQ4" s="75"/>
-      <c r="AR4" s="75"/>
-      <c r="AS4" s="75"/>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="75"/>
-      <c r="AY4" s="75"/>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="75"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="75"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="75"/>
-      <c r="BF4" s="76"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="50"/>
+      <c r="AC4" s="50"/>
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="50"/>
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="50"/>
+      <c r="AJ4" s="50"/>
+      <c r="AK4" s="50"/>
+      <c r="AL4" s="50"/>
+      <c r="AM4" s="50"/>
+      <c r="AN4" s="50"/>
+      <c r="AO4" s="50"/>
+      <c r="AP4" s="50"/>
+      <c r="AQ4" s="50"/>
+      <c r="AR4" s="50"/>
+      <c r="AS4" s="50"/>
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="50"/>
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="50"/>
+      <c r="AZ4" s="50"/>
+      <c r="BA4" s="50"/>
+      <c r="BB4" s="50"/>
+      <c r="BC4" s="50"/>
+      <c r="BD4" s="50"/>
+      <c r="BE4" s="50"/>
+      <c r="BF4" s="51"/>
     </row>
     <row r="5" spans="2:58" ht="30" customHeight="1">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -16745,12 +16762,12 @@
       <c r="BF5" s="9"/>
     </row>
     <row r="6" spans="2:58" ht="51" customHeight="1">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -16806,12 +16823,12 @@
       <c r="BF6" s="16"/>
     </row>
     <row r="7" spans="2:58" ht="45.75" customHeight="1">
-      <c r="B7" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74"/>
+      <c r="B7" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -16867,12 +16884,12 @@
       <c r="BF7" s="14"/>
     </row>
     <row r="8" spans="2:58" ht="63.75" customHeight="1">
-      <c r="B8" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="74"/>
+      <c r="B8" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="32"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
@@ -16928,12 +16945,12 @@
       <c r="BF8" s="31"/>
     </row>
     <row r="9" spans="2:58" ht="54" customHeight="1">
-      <c r="B9" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
+      <c r="B9" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="38"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
@@ -16989,12 +17006,12 @@
       <c r="BF9" s="41"/>
     </row>
     <row r="10" spans="2:58" ht="28.5" customHeight="1">
-      <c r="B10" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="74"/>
+      <c r="B10" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="38"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
@@ -17050,12 +17067,12 @@
       <c r="BF10" s="41"/>
     </row>
     <row r="11" spans="2:58" ht="36" customHeight="1">
-      <c r="B11" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="74"/>
+      <c r="B11" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="32"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
@@ -17112,12 +17129,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F4:BF4"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:BF1"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
@@ -17129,6 +17140,12 @@
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F4:BF4"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17153,10 +17170,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
         <v>95</v>
-      </c>
-      <c r="B1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -17164,7 +17181,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -17172,7 +17189,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -17180,7 +17197,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -17188,7 +17205,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -17199,1237 +17216,1772 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="20"/>
-    <col min="2" max="2" width="13.375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="23.75" style="28" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="21"/>
+    <col min="2" max="2" width="16.75" style="21" customWidth="1"/>
+    <col min="3" max="3" width="13.375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="23.75" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>127</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="20">
         <v>176</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="23">
+        <v>41407</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="20">
         <v>175</v>
       </c>
-      <c r="B3" s="23"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" s="23">
+        <v>41414</v>
+      </c>
+      <c r="C3" s="23"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="20">
         <v>174</v>
       </c>
-      <c r="B4" s="23"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4" s="23">
+        <v>41421</v>
+      </c>
+      <c r="C4" s="23"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="20">
         <v>173</v>
       </c>
-      <c r="B5" s="23"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" s="23">
+        <v>41428</v>
+      </c>
+      <c r="C5" s="23"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="20">
         <v>172</v>
       </c>
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" s="23">
+        <v>41435</v>
+      </c>
+      <c r="C6" s="23"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="20">
         <v>171</v>
       </c>
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7" s="23">
+        <v>41442</v>
+      </c>
+      <c r="C7" s="23"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="20">
         <v>170</v>
       </c>
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" s="23">
+        <v>41449</v>
+      </c>
+      <c r="C8" s="23"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="20">
         <v>169</v>
       </c>
-      <c r="B9" s="23"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="B9" s="23">
+        <v>41456</v>
+      </c>
+      <c r="C9" s="23"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="20">
         <v>168</v>
       </c>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="23">
+        <v>41463</v>
+      </c>
+      <c r="C10" s="23"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="20">
         <v>167</v>
       </c>
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="B11" s="23">
+        <v>41470</v>
+      </c>
+      <c r="C11" s="23"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="20">
         <v>166</v>
       </c>
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12" s="23">
+        <v>41477</v>
+      </c>
+      <c r="C12" s="23"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="20">
         <v>165</v>
       </c>
-      <c r="B13" s="23"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="B13" s="23">
+        <v>41484</v>
+      </c>
+      <c r="C13" s="23"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="20">
         <v>164</v>
       </c>
-      <c r="B14" s="23"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="B14" s="23">
+        <v>41491</v>
+      </c>
+      <c r="C14" s="23"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="20">
         <v>163</v>
       </c>
-      <c r="B15" s="23"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="23">
+        <v>41498</v>
+      </c>
+      <c r="C15" s="23"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="20">
         <v>162</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="B16" s="23">
+        <v>41505</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="20">
         <v>161</v>
       </c>
-      <c r="B17" s="23"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="B17" s="23">
+        <v>41512</v>
+      </c>
+      <c r="C17" s="23"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="20">
         <v>160</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="B18" s="23">
+        <v>41519</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="20">
         <v>159</v>
       </c>
-      <c r="B19" s="23"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="B19" s="23">
+        <v>41526</v>
+      </c>
+      <c r="C19" s="23"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="20">
         <v>158</v>
       </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="B20" s="23">
+        <v>41533</v>
+      </c>
+      <c r="C20" s="23"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="20">
         <v>157</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="26"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="B21" s="23">
+        <v>41540</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="20">
         <v>156</v>
       </c>
-      <c r="B22" s="23"/>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="B22" s="23">
+        <v>41547</v>
+      </c>
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="20">
         <v>155</v>
       </c>
-      <c r="B23" s="23"/>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="B23" s="23">
+        <v>41554</v>
+      </c>
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="20">
         <v>154</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="B24" s="23">
+        <v>41561</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="20">
         <v>153</v>
       </c>
-      <c r="B25" s="23"/>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="B25" s="23">
+        <v>41568</v>
+      </c>
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="20">
         <v>152</v>
       </c>
-      <c r="B26" s="23"/>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="B26" s="23">
+        <v>41575</v>
+      </c>
+      <c r="C26" s="23"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="20">
         <v>151</v>
       </c>
-      <c r="B27" s="23"/>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="B27" s="23">
+        <v>41582</v>
+      </c>
+      <c r="C27" s="23"/>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="20">
         <v>150</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="26"/>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="B28" s="23">
+        <v>41589</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="20">
         <v>149</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="26"/>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="B29" s="23">
+        <v>41596</v>
+      </c>
+      <c r="C29" s="23"/>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="20">
         <v>148</v>
       </c>
-      <c r="B30" s="23"/>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="B30" s="23">
+        <v>41603</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="20">
         <v>147</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="B31" s="23">
+        <v>41610</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="20">
         <v>146</v>
       </c>
-      <c r="B32" s="23"/>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="B32" s="23">
+        <v>41617</v>
+      </c>
+      <c r="C32" s="23"/>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="20">
         <v>145</v>
       </c>
-      <c r="B33" s="23"/>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="B33" s="23">
+        <v>41624</v>
+      </c>
+      <c r="C33" s="23"/>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="20">
         <v>144</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="26"/>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="B34" s="23">
+        <v>41631</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="20">
         <v>143</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="B35" s="23">
+        <v>41638</v>
+      </c>
+      <c r="C35" s="23"/>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="20">
         <v>142</v>
       </c>
-      <c r="B36" s="23"/>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="B36" s="23">
+        <v>41645</v>
+      </c>
+      <c r="C36" s="23"/>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="20">
         <v>141</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="B37" s="23">
+        <v>41652</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="20">
         <v>140</v>
       </c>
-      <c r="B38" s="23"/>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="B38" s="23">
+        <v>41659</v>
+      </c>
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="20">
         <v>139</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="26"/>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="B39" s="23">
+        <v>41666</v>
+      </c>
+      <c r="C39" s="23"/>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="20">
         <v>138</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="B40" s="23">
+        <v>41673</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="D40" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="20">
         <v>137</v>
       </c>
-      <c r="B41" s="23"/>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1">
+      <c r="B41" s="23">
+        <v>41680</v>
+      </c>
+      <c r="C41" s="23"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="20">
         <v>136</v>
       </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="B42" s="23">
+        <v>41687</v>
+      </c>
+      <c r="C42" s="23"/>
+      <c r="D42" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="20">
         <v>135</v>
       </c>
-      <c r="B43" s="23"/>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="B43" s="23">
+        <v>41694</v>
+      </c>
+      <c r="C43" s="23"/>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="20">
         <v>134</v>
       </c>
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="B44" s="23">
+        <v>41701</v>
+      </c>
+      <c r="C44" s="23"/>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="20">
         <v>133</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="26"/>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="B45" s="23">
+        <v>41708</v>
+      </c>
+      <c r="C45" s="23"/>
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="20">
         <v>132</v>
       </c>
-      <c r="B46" s="23"/>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="B46" s="23">
+        <v>41715</v>
+      </c>
+      <c r="C46" s="23"/>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="20">
         <v>131</v>
       </c>
-      <c r="B47" s="23"/>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="B47" s="23">
+        <v>41722</v>
+      </c>
+      <c r="C47" s="23"/>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="20">
         <v>130</v>
       </c>
-      <c r="B48" s="23"/>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="B48" s="23">
+        <v>41729</v>
+      </c>
+      <c r="C48" s="23"/>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="20">
         <v>129</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="26"/>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="B49" s="23">
+        <v>41736</v>
+      </c>
+      <c r="C49" s="23"/>
+      <c r="D49" s="26"/>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="20">
         <v>128</v>
       </c>
-      <c r="B50" s="23"/>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="B50" s="23">
+        <v>41743</v>
+      </c>
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="20">
         <v>127</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="B51" s="23">
+        <v>41750</v>
+      </c>
+      <c r="C51" s="23"/>
+      <c r="D51" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="20">
         <v>126</v>
       </c>
-      <c r="B52" s="23"/>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="B52" s="23">
+        <v>41757</v>
+      </c>
+      <c r="C52" s="23"/>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="20">
         <v>125</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="26"/>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="B53" s="23">
+        <v>41764</v>
+      </c>
+      <c r="C53" s="23"/>
+      <c r="D53" s="26"/>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="20">
         <v>124</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="B54" s="23">
+        <v>41771</v>
+      </c>
+      <c r="C54" s="23"/>
+      <c r="D54" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="20">
         <v>123</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="29"/>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="B55" s="23">
+        <v>41778</v>
+      </c>
+      <c r="C55" s="23"/>
+      <c r="D55" s="29"/>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="20">
         <v>122</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="26"/>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="B56" s="23">
+        <v>41785</v>
+      </c>
+      <c r="C56" s="23"/>
+      <c r="D56" s="26"/>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="20">
         <v>121</v>
       </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="B57" s="23">
+        <v>41792</v>
+      </c>
+      <c r="C57" s="23"/>
+      <c r="D57" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="20">
         <v>120</v>
       </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="B58" s="23">
+        <v>41799</v>
+      </c>
+      <c r="C58" s="23"/>
+      <c r="D58" s="29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="20">
         <v>119</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="26"/>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="B59" s="23">
+        <v>41806</v>
+      </c>
+      <c r="C59" s="23"/>
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="20">
         <v>118</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="B60" s="23">
+        <v>41813</v>
+      </c>
+      <c r="C60" s="23"/>
+      <c r="D60" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="20">
         <v>117</v>
       </c>
-      <c r="B61" s="23"/>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="B61" s="23">
+        <v>41820</v>
+      </c>
+      <c r="C61" s="23"/>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="20">
         <v>116</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="B62" s="23">
+        <v>41827</v>
+      </c>
+      <c r="C62" s="23"/>
+      <c r="D62" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="20">
         <v>115</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="26"/>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="B63" s="23">
+        <v>41834</v>
+      </c>
+      <c r="C63" s="23"/>
+      <c r="D63" s="26"/>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="20">
         <v>114</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="B64" s="23">
+        <v>41841</v>
+      </c>
+      <c r="C64" s="23"/>
+      <c r="D64" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="20">
         <v>113</v>
       </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="26"/>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="B65" s="23">
+        <v>41848</v>
+      </c>
+      <c r="C65" s="23"/>
+      <c r="D65" s="26"/>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="20">
         <v>112</v>
       </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="26"/>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="B66" s="23">
+        <v>41855</v>
+      </c>
+      <c r="C66" s="23"/>
+      <c r="D66" s="26"/>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="20">
         <v>111</v>
       </c>
-      <c r="B67" s="23"/>
-      <c r="C67" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="B67" s="23">
+        <v>41862</v>
+      </c>
+      <c r="C67" s="23"/>
+      <c r="D67" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="20">
         <v>110</v>
       </c>
-      <c r="B68" s="23"/>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="B68" s="23">
+        <v>41869</v>
+      </c>
+      <c r="C68" s="23"/>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="20">
         <v>109</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="26"/>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="B69" s="23">
+        <v>41876</v>
+      </c>
+      <c r="C69" s="23"/>
+      <c r="D69" s="26"/>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="20">
         <v>108</v>
       </c>
-      <c r="B70" s="23"/>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="B70" s="23">
+        <v>41883</v>
+      </c>
+      <c r="C70" s="23"/>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="20">
         <v>107</v>
       </c>
-      <c r="B71" s="23"/>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="B71" s="23">
+        <v>41890</v>
+      </c>
+      <c r="C71" s="23"/>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="20">
         <v>106</v>
       </c>
-      <c r="B72" s="23"/>
-    </row>
-    <row r="73" spans="1:3" ht="25.5">
+      <c r="B72" s="23">
+        <v>41897</v>
+      </c>
+      <c r="C72" s="23"/>
+    </row>
+    <row r="73" spans="1:4" ht="25.5">
       <c r="A73" s="20">
         <v>105</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="B73" s="23">
+        <v>41904</v>
+      </c>
+      <c r="C73" s="23"/>
+      <c r="D73" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="20">
         <v>104</v>
       </c>
-      <c r="B74" s="23"/>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="B74" s="23">
+        <v>41911</v>
+      </c>
+      <c r="C74" s="23"/>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="20">
         <v>103</v>
       </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="26"/>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="B75" s="23">
+        <v>41918</v>
+      </c>
+      <c r="C75" s="23"/>
+      <c r="D75" s="26"/>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="20">
         <v>102</v>
       </c>
-      <c r="B76" s="23"/>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="B76" s="23">
+        <v>41925</v>
+      </c>
+      <c r="C76" s="23"/>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="20">
         <v>101</v>
       </c>
-      <c r="B77" s="23"/>
-      <c r="C77" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="B77" s="23">
+        <v>41932</v>
+      </c>
+      <c r="C77" s="23"/>
+      <c r="D77" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="20">
         <v>100</v>
       </c>
-      <c r="B78" s="23"/>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="B78" s="23">
+        <v>41939</v>
+      </c>
+      <c r="C78" s="23"/>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="20">
         <v>99</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="26"/>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="B79" s="23">
+        <v>41946</v>
+      </c>
+      <c r="C79" s="23"/>
+      <c r="D79" s="26"/>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="20">
         <v>98</v>
       </c>
-      <c r="B80" s="23"/>
-      <c r="C80" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="B80" s="23">
+        <v>41953</v>
+      </c>
+      <c r="C80" s="23"/>
+      <c r="D80" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="20">
         <v>97</v>
       </c>
-      <c r="B81" s="23"/>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="B81" s="23">
+        <v>41960</v>
+      </c>
+      <c r="C81" s="23"/>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="20">
         <v>96</v>
       </c>
-      <c r="B82" s="23"/>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="B82" s="23">
+        <v>41967</v>
+      </c>
+      <c r="C82" s="23"/>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="20">
         <v>95</v>
       </c>
-      <c r="B83" s="23"/>
-    </row>
-    <row r="84" spans="1:3" ht="25.5">
+      <c r="B83" s="23">
+        <v>41974</v>
+      </c>
+      <c r="C83" s="23"/>
+    </row>
+    <row r="84" spans="1:4" ht="25.5">
       <c r="A84" s="20">
         <v>94</v>
       </c>
-      <c r="B84" s="23"/>
-      <c r="C84" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="B84" s="23">
+        <v>41981</v>
+      </c>
+      <c r="C84" s="23"/>
+      <c r="D84" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="20">
         <v>93</v>
       </c>
-      <c r="B85" s="23"/>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="B85" s="23">
+        <v>41988</v>
+      </c>
+      <c r="C85" s="23"/>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="20">
         <v>92</v>
       </c>
-      <c r="B86" s="23"/>
-      <c r="C86" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="B86" s="23">
+        <v>41995</v>
+      </c>
+      <c r="C86" s="23"/>
+      <c r="D86" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="20">
         <v>91</v>
       </c>
-      <c r="B87" s="23"/>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="B87" s="23">
+        <v>42002</v>
+      </c>
+      <c r="C87" s="23"/>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="20">
         <v>90</v>
       </c>
-      <c r="B88" s="23"/>
-      <c r="C88" s="26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="B88" s="23">
+        <v>42009</v>
+      </c>
+      <c r="C88" s="23"/>
+      <c r="D88" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="20">
         <v>89</v>
       </c>
-      <c r="B89" s="23"/>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="B89" s="23">
+        <v>42016</v>
+      </c>
+      <c r="C89" s="23"/>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="20">
         <v>88</v>
       </c>
-      <c r="B90" s="23"/>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="B90" s="23">
+        <v>42023</v>
+      </c>
+      <c r="C90" s="23"/>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="20">
         <v>87</v>
       </c>
-      <c r="B91" s="23"/>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="B91" s="23">
+        <v>42030</v>
+      </c>
+      <c r="C91" s="23"/>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="20">
         <v>86</v>
       </c>
-      <c r="B92" s="23"/>
-      <c r="C92" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="B92" s="23">
+        <v>42037</v>
+      </c>
+      <c r="C92" s="23"/>
+      <c r="D92" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="20">
         <v>85</v>
       </c>
-      <c r="B93" s="23"/>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="B93" s="23">
+        <v>42044</v>
+      </c>
+      <c r="C93" s="23"/>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="20">
         <v>84</v>
       </c>
-      <c r="B94" s="23"/>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="B94" s="23">
+        <v>42051</v>
+      </c>
+      <c r="C94" s="23"/>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="20">
         <v>83</v>
       </c>
-      <c r="B95" s="23"/>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="B95" s="23">
+        <v>42058</v>
+      </c>
+      <c r="C95" s="23"/>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="20">
         <v>82</v>
       </c>
-      <c r="B96" s="23"/>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="B96" s="23">
+        <v>42065</v>
+      </c>
+      <c r="C96" s="23"/>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="20">
         <v>81</v>
       </c>
-      <c r="B97" s="23"/>
-      <c r="C97" s="26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="B97" s="23">
+        <v>42072</v>
+      </c>
+      <c r="C97" s="23"/>
+      <c r="D97" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="20">
         <v>80</v>
       </c>
-      <c r="B98" s="23"/>
-      <c r="C98" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="B98" s="23">
+        <v>42079</v>
+      </c>
+      <c r="C98" s="23"/>
+      <c r="D98" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="20">
         <v>79</v>
       </c>
-      <c r="B99" s="23"/>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="B99" s="23">
+        <v>42086</v>
+      </c>
+      <c r="C99" s="23"/>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="20">
         <v>78</v>
       </c>
-      <c r="B100" s="23"/>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="B100" s="23">
+        <v>42093</v>
+      </c>
+      <c r="C100" s="23"/>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="20">
         <v>77</v>
       </c>
-      <c r="B101" s="23"/>
-      <c r="C101" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="B101" s="23">
+        <v>42100</v>
+      </c>
+      <c r="C101" s="23"/>
+      <c r="D101" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="20">
         <v>76</v>
       </c>
-      <c r="B102" s="23"/>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="B102" s="23">
+        <v>42107</v>
+      </c>
+      <c r="C102" s="23"/>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="20">
         <v>75</v>
       </c>
-      <c r="B103" s="23"/>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="B103" s="23">
+        <v>42114</v>
+      </c>
+      <c r="C103" s="23"/>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="20">
         <v>74</v>
       </c>
-      <c r="B104" s="23"/>
-      <c r="C104" s="26"/>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="B104" s="23">
+        <v>42121</v>
+      </c>
+      <c r="C104" s="23"/>
+      <c r="D104" s="26"/>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" s="20">
         <v>73</v>
       </c>
-      <c r="B105" s="23"/>
-      <c r="C105" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="B105" s="23">
+        <v>42128</v>
+      </c>
+      <c r="C105" s="23"/>
+      <c r="D105" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="20">
         <v>72</v>
       </c>
-      <c r="B106" s="23"/>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="B106" s="23">
+        <v>42135</v>
+      </c>
+      <c r="C106" s="23"/>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="20">
         <v>71</v>
       </c>
-      <c r="B107" s="23"/>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="B107" s="23">
+        <v>42142</v>
+      </c>
+      <c r="C107" s="23"/>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="20">
         <v>70</v>
       </c>
-      <c r="B108" s="23"/>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="B108" s="23">
+        <v>42149</v>
+      </c>
+      <c r="C108" s="23"/>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="20">
         <v>69</v>
       </c>
-      <c r="B109" s="23"/>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="B109" s="23">
+        <v>42156</v>
+      </c>
+      <c r="C109" s="23"/>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="20">
         <v>68</v>
       </c>
-      <c r="B110" s="23"/>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="B110" s="23">
+        <v>42163</v>
+      </c>
+      <c r="C110" s="23"/>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" s="20">
         <v>67</v>
       </c>
-      <c r="B111" s="23"/>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="B111" s="23">
+        <v>42170</v>
+      </c>
+      <c r="C111" s="23"/>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="20">
         <v>66</v>
       </c>
-      <c r="B112" s="23"/>
-    </row>
-    <row r="113" spans="1:3" ht="25.5">
+      <c r="B112" s="23">
+        <v>42177</v>
+      </c>
+      <c r="C112" s="23"/>
+    </row>
+    <row r="113" spans="1:4" ht="25.5">
       <c r="A113" s="20">
         <v>65</v>
       </c>
-      <c r="B113" s="23"/>
-      <c r="C113" s="27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="B113" s="23">
+        <v>42184</v>
+      </c>
+      <c r="C113" s="23"/>
+      <c r="D113" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="20">
         <v>64</v>
       </c>
-      <c r="B114" s="23"/>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="B114" s="23">
+        <v>42191</v>
+      </c>
+      <c r="C114" s="23"/>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="20">
         <v>63</v>
       </c>
-      <c r="B115" s="23"/>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="B115" s="23">
+        <v>42198</v>
+      </c>
+      <c r="C115" s="23"/>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="20">
         <v>62</v>
       </c>
-      <c r="B116" s="23"/>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="B116" s="23">
+        <v>42205</v>
+      </c>
+      <c r="C116" s="23"/>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="20">
         <v>61</v>
       </c>
-      <c r="B117" s="23"/>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="B117" s="23">
+        <v>42212</v>
+      </c>
+      <c r="C117" s="23"/>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="20">
         <v>60</v>
       </c>
-      <c r="B118" s="23"/>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="B118" s="23">
+        <v>42219</v>
+      </c>
+      <c r="C118" s="23"/>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="20">
         <v>59</v>
       </c>
-      <c r="B119" s="23"/>
-      <c r="C119" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="B119" s="23">
+        <v>42226</v>
+      </c>
+      <c r="C119" s="23"/>
+      <c r="D119" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="20">
         <v>58</v>
       </c>
-      <c r="B120" s="23"/>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="B120" s="23">
+        <v>42233</v>
+      </c>
+      <c r="C120" s="23"/>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="20">
         <v>57</v>
       </c>
-      <c r="B121" s="23"/>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="B121" s="23">
+        <v>42240</v>
+      </c>
+      <c r="C121" s="23"/>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="20">
         <v>56</v>
       </c>
-      <c r="B122" s="23"/>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="B122" s="23">
+        <v>42247</v>
+      </c>
+      <c r="C122" s="23"/>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="20">
         <v>55</v>
       </c>
-      <c r="B123" s="23"/>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="B123" s="23">
+        <v>42254</v>
+      </c>
+      <c r="C123" s="23"/>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="20">
         <v>54</v>
       </c>
-      <c r="B124" s="23"/>
-    </row>
-    <row r="125" spans="1:3" ht="25.5">
+      <c r="B124" s="23">
+        <v>42261</v>
+      </c>
+      <c r="C124" s="23"/>
+    </row>
+    <row r="125" spans="1:4" ht="25.5">
       <c r="A125" s="20">
         <v>53</v>
       </c>
-      <c r="B125" s="23"/>
-      <c r="C125" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="B125" s="23">
+        <v>42268</v>
+      </c>
+      <c r="C125" s="23"/>
+      <c r="D125" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="20">
         <v>52</v>
       </c>
-      <c r="B126" s="23"/>
-    </row>
-    <row r="127" spans="1:3" ht="19.5" customHeight="1">
+      <c r="B126" s="23">
+        <v>42275</v>
+      </c>
+      <c r="C126" s="23"/>
+    </row>
+    <row r="127" spans="1:4" ht="19.5" customHeight="1">
       <c r="A127" s="20">
         <v>51</v>
       </c>
-      <c r="B127" s="23"/>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="B127" s="23">
+        <v>42282</v>
+      </c>
+      <c r="C127" s="23"/>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="20">
         <v>50</v>
       </c>
-      <c r="B128" s="23"/>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="B128" s="23">
+        <v>42289</v>
+      </c>
+      <c r="C128" s="23"/>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="20">
         <v>49</v>
       </c>
-      <c r="B129" s="23"/>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="B129" s="23">
+        <v>42296</v>
+      </c>
+      <c r="C129" s="23"/>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="20">
         <v>48</v>
       </c>
-      <c r="B130" s="23"/>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="B130" s="23">
+        <v>42303</v>
+      </c>
+      <c r="C130" s="23"/>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="20">
         <v>47</v>
       </c>
-      <c r="B131" s="23"/>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="B131" s="23">
+        <v>42310</v>
+      </c>
+      <c r="C131" s="23"/>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="20">
         <v>46</v>
       </c>
-      <c r="B132" s="23"/>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="B132" s="23">
+        <v>42317</v>
+      </c>
+      <c r="C132" s="23"/>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="20">
         <v>45</v>
       </c>
-      <c r="B133" s="23"/>
-      <c r="C133" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="B133" s="23">
+        <v>42324</v>
+      </c>
+      <c r="C133" s="23"/>
+      <c r="D133" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="20">
         <v>44</v>
       </c>
-      <c r="B134" s="23"/>
-      <c r="C134" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="B134" s="23">
+        <v>42331</v>
+      </c>
+      <c r="C134" s="23"/>
+      <c r="D134" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="20">
         <v>43</v>
       </c>
-      <c r="B135" s="23"/>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="B135" s="23">
+        <v>42338</v>
+      </c>
+      <c r="C135" s="23"/>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="20">
         <v>42</v>
       </c>
-      <c r="B136" s="23"/>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="B136" s="23">
+        <v>42345</v>
+      </c>
+      <c r="C136" s="23"/>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="20">
         <v>41</v>
       </c>
-      <c r="B137" s="23"/>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="B137" s="23">
+        <v>42352</v>
+      </c>
+      <c r="C137" s="23"/>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="20">
         <v>40</v>
       </c>
-      <c r="B138" s="23"/>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="B138" s="23">
+        <v>42359</v>
+      </c>
+      <c r="C138" s="23"/>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="20">
         <v>39</v>
       </c>
-      <c r="B139" s="23"/>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="B139" s="23">
+        <v>42366</v>
+      </c>
+      <c r="C139" s="23"/>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="20">
         <v>38</v>
       </c>
-      <c r="B140" s="23"/>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="B140" s="23">
+        <v>42373</v>
+      </c>
+      <c r="C140" s="23"/>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="20">
         <v>37</v>
       </c>
-      <c r="B141" s="23"/>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="B141" s="23">
+        <v>42380</v>
+      </c>
+      <c r="C141" s="23"/>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="20">
         <v>36</v>
       </c>
-      <c r="B142" s="23"/>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="B142" s="23">
+        <v>42387</v>
+      </c>
+      <c r="C142" s="23"/>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="20">
         <v>35</v>
       </c>
-      <c r="B143" s="23"/>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="B143" s="23">
+        <v>42394</v>
+      </c>
+      <c r="C143" s="23"/>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="20">
         <v>34</v>
       </c>
-      <c r="B144" s="23"/>
-      <c r="C144" s="26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="B144" s="23">
+        <v>42401</v>
+      </c>
+      <c r="C144" s="23"/>
+      <c r="D144" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="20">
         <v>33</v>
       </c>
-      <c r="B145" s="23"/>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="B145" s="23">
+        <v>42408</v>
+      </c>
+      <c r="C145" s="23"/>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="20">
         <v>32</v>
       </c>
-      <c r="B146" s="23"/>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="B146" s="23">
+        <v>42415</v>
+      </c>
+      <c r="C146" s="23"/>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="20">
         <v>31</v>
       </c>
-      <c r="B147" s="23"/>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="B147" s="23">
+        <v>42422</v>
+      </c>
+      <c r="C147" s="23"/>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="20">
         <v>30</v>
       </c>
-      <c r="B148" s="23"/>
-      <c r="C148" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="B148" s="23">
+        <v>42429</v>
+      </c>
+      <c r="C148" s="23"/>
+      <c r="D148" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="20">
         <v>29</v>
       </c>
-      <c r="B149" s="23"/>
-      <c r="C149" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="B149" s="23">
+        <v>42436</v>
+      </c>
+      <c r="C149" s="23"/>
+      <c r="D149" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="20">
         <v>28</v>
       </c>
-      <c r="B150" s="23"/>
-    </row>
-    <row r="151" spans="1:3">
+      <c r="B150" s="23">
+        <v>42443</v>
+      </c>
+      <c r="C150" s="23"/>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="20">
         <v>27</v>
       </c>
-      <c r="B151" s="23"/>
-    </row>
-    <row r="152" spans="1:3">
+      <c r="B151" s="23">
+        <v>42450</v>
+      </c>
+      <c r="C151" s="23"/>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="20">
         <v>26</v>
       </c>
-      <c r="B152" s="23"/>
-    </row>
-    <row r="153" spans="1:3">
+      <c r="B152" s="23">
+        <v>42457</v>
+      </c>
+      <c r="C152" s="23"/>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="20">
         <v>25</v>
       </c>
-      <c r="B153" s="23"/>
-      <c r="C153" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
+      <c r="B153" s="23">
+        <v>42464</v>
+      </c>
+      <c r="C153" s="23"/>
+      <c r="D153" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="20">
         <v>24</v>
       </c>
-      <c r="B154" s="23"/>
-    </row>
-    <row r="155" spans="1:3">
+      <c r="B154" s="23">
+        <v>42471</v>
+      </c>
+      <c r="C154" s="23"/>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="20">
         <v>23</v>
       </c>
-      <c r="B155" s="23"/>
-    </row>
-    <row r="156" spans="1:3">
+      <c r="B155" s="23">
+        <v>42478</v>
+      </c>
+      <c r="C155" s="23"/>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="20">
         <v>22</v>
       </c>
-      <c r="B156" s="23"/>
-    </row>
-    <row r="157" spans="1:3" ht="24" customHeight="1">
+      <c r="B156" s="23">
+        <v>42485</v>
+      </c>
+      <c r="C156" s="23"/>
+    </row>
+    <row r="157" spans="1:4" ht="24" customHeight="1">
       <c r="A157" s="20">
         <v>21</v>
       </c>
-      <c r="B157" s="23"/>
-      <c r="C157" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
+      <c r="B157" s="23">
+        <v>42492</v>
+      </c>
+      <c r="C157" s="23"/>
+      <c r="D157" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="20">
         <v>20</v>
       </c>
-      <c r="B158" s="23"/>
-    </row>
-    <row r="159" spans="1:3">
+      <c r="B158" s="23">
+        <v>42499</v>
+      </c>
+      <c r="C158" s="23"/>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="20">
         <v>19</v>
       </c>
-      <c r="B159" s="23"/>
-    </row>
-    <row r="160" spans="1:3">
+      <c r="B159" s="23">
+        <v>42506</v>
+      </c>
+      <c r="C159" s="23"/>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="20">
         <v>18</v>
       </c>
-      <c r="B160" s="23"/>
-    </row>
-    <row r="161" spans="1:3">
+      <c r="B160" s="23">
+        <v>42513</v>
+      </c>
+      <c r="C160" s="23"/>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="20">
         <v>17</v>
       </c>
-      <c r="B161" s="23"/>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="B161" s="23">
+        <v>42520</v>
+      </c>
+      <c r="C161" s="23"/>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="20">
         <v>16</v>
       </c>
-      <c r="B162" s="23"/>
-    </row>
-    <row r="163" spans="1:3">
+      <c r="B162" s="23">
+        <v>42527</v>
+      </c>
+      <c r="C162" s="23"/>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="20">
         <v>15</v>
       </c>
-      <c r="B163" s="23"/>
-    </row>
-    <row r="164" spans="1:3">
+      <c r="B163" s="23">
+        <v>42534</v>
+      </c>
+      <c r="C163" s="23"/>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="20">
         <v>14</v>
       </c>
-      <c r="B164" s="23"/>
-      <c r="C164" s="26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+      <c r="B164" s="23">
+        <v>42541</v>
+      </c>
+      <c r="C164" s="23"/>
+      <c r="D164" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="20">
         <v>13</v>
       </c>
-      <c r="B165" s="23"/>
-      <c r="C165" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="B165" s="23">
+        <v>42548</v>
+      </c>
+      <c r="C165" s="23"/>
+      <c r="D165" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="20">
         <v>12</v>
       </c>
-      <c r="B166" s="23"/>
-      <c r="C166" s="26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
+      <c r="B166" s="23">
+        <v>42555</v>
+      </c>
+      <c r="C166" s="23"/>
+      <c r="D166" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" s="20">
         <v>11</v>
       </c>
-      <c r="B167" s="23"/>
-      <c r="C167" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+      <c r="B167" s="23">
+        <v>42562</v>
+      </c>
+      <c r="C167" s="23"/>
+      <c r="D167" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" s="20">
         <v>10</v>
       </c>
-      <c r="B168" s="23"/>
-      <c r="C168" s="26"/>
-    </row>
-    <row r="169" spans="1:3">
+      <c r="B168" s="23">
+        <v>42569</v>
+      </c>
+      <c r="C168" s="23"/>
+      <c r="D168" s="26"/>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" s="20">
         <v>9</v>
       </c>
-      <c r="B169" s="23"/>
-    </row>
-    <row r="170" spans="1:3">
+      <c r="B169" s="23">
+        <v>42576</v>
+      </c>
+      <c r="C169" s="23"/>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" s="20">
         <v>8</v>
       </c>
-      <c r="B170" s="23"/>
-    </row>
-    <row r="171" spans="1:3">
+      <c r="B170" s="23">
+        <v>42583</v>
+      </c>
+      <c r="C170" s="23"/>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" s="20">
         <v>7</v>
       </c>
-      <c r="B171" s="23"/>
-    </row>
-    <row r="172" spans="1:3">
+      <c r="B171" s="23">
+        <v>42590</v>
+      </c>
+      <c r="C171" s="23"/>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" s="20">
         <v>6</v>
       </c>
-      <c r="B172" s="23"/>
-    </row>
-    <row r="173" spans="1:3">
+      <c r="B172" s="23">
+        <v>42597</v>
+      </c>
+      <c r="C172" s="23"/>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="20">
         <v>5</v>
       </c>
-      <c r="B173" s="23"/>
-    </row>
-    <row r="174" spans="1:3">
+      <c r="B173" s="23">
+        <v>42604</v>
+      </c>
+      <c r="C173" s="23"/>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="20">
         <v>4</v>
       </c>
-      <c r="B174" s="23"/>
-    </row>
-    <row r="175" spans="1:3">
+      <c r="B174" s="23">
+        <v>42611</v>
+      </c>
+      <c r="C174" s="23"/>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" s="20">
         <v>3</v>
       </c>
-      <c r="B175" s="23"/>
-    </row>
-    <row r="176" spans="1:3">
+      <c r="B175" s="23">
+        <v>42618</v>
+      </c>
+      <c r="C175" s="23"/>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="20">
         <v>2</v>
       </c>
-      <c r="B176" s="23"/>
-    </row>
-    <row r="177" spans="1:3">
+      <c r="B176" s="23">
+        <v>42625</v>
+      </c>
+      <c r="C176" s="23"/>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="20">
         <v>1</v>
       </c>
-      <c r="B177" s="23"/>
-    </row>
-    <row r="178" spans="1:3">
+      <c r="B177" s="23">
+        <v>42632</v>
+      </c>
+      <c r="C177" s="23"/>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="20">
         <v>0</v>
       </c>
-      <c r="B178" s="23"/>
-      <c r="C178" s="26" t="s">
-        <v>50</v>
+      <c r="B178" s="23">
+        <v>42641</v>
+      </c>
+      <c r="C178" s="23"/>
+      <c r="D178" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -18444,7 +18996,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18454,22 +19006,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -18483,7 +19035,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18494,23 +19046,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="23">
         <v>42503</v>
@@ -18518,7 +19070,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="23">
         <v>42534</v>
@@ -18526,15 +19078,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>89</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -18542,10 +19094,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
         <v>97</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -18558,8 +19110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18570,23 +19122,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="23">
         <v>42564</v>
@@ -18594,7 +19146,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="23">
         <v>42595</v>
@@ -18602,15 +19154,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -18618,34 +19170,34 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -18656,10 +19208,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18670,23 +19222,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="23">
         <v>42626</v>
@@ -18694,7 +19246,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="23">
         <v>42656</v>
@@ -18702,50 +19254,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B10" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -18769,23 +19289,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="23">
         <v>42687</v>
@@ -18793,7 +19313,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="23">
         <v>42717</v>
@@ -18801,15 +19321,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -18826,7 +19346,7 @@
   <dimension ref="A1:F259"/>
   <sheetViews>
     <sheetView topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="F239" sqref="F239"/>
+      <selection activeCell="K258" sqref="K258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18834,64 +19354,64 @@
     <row r="1" spans="1:6" ht="15">
       <c r="A1" s="43"/>
       <c r="B1" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="15">
       <c r="A2" s="43"/>
       <c r="B2" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="43"/>
       <c r="B3" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="D3" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="E3" s="43" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>106</v>
       </c>
       <c r="F3" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="43"/>
       <c r="B4" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="44"/>
     </row>
@@ -18905,55 +19425,55 @@
     </row>
     <row r="6" spans="1:6" ht="15">
       <c r="A6" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>108</v>
-      </c>
       <c r="C6" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F6" s="44"/>
     </row>
     <row r="7" spans="1:6" ht="15">
       <c r="A7" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>110</v>
-      </c>
       <c r="C7" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" s="44"/>
     </row>
     <row r="8" spans="1:6" ht="15">
       <c r="A8" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="D8" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="E8" s="43" t="s">
         <v>105</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>106</v>
       </c>
       <c r="F8" s="44"/>
     </row>
@@ -23296,12 +23816,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>